<commit_message>
unit test for chequing_account.py
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_chequing_account.xlsx
+++ b/tests/A02_pixell_test_plan_chequing_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\assignments\assignment_02\instructions\given_files\assignment_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c3d6174ceab06f3/Desktop/rrc_polytech/courses_term2/intermediate_software_development/project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C62CC4-BE0A-4A80-805F-8E9765287A3B}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3555" windowWidth="25185" windowHeight="11415" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,13 +249,466 @@
   </si>
   <si>
     <t>Attributes are set to input values (ensure to test for superclass and subclass attributes)</t>
+  </si>
+  <si>
+    <t>Jashanpreet Kaur Jattana</t>
+  </si>
+  <si>
+    <t>A valid account number, client number, balance, and overdraft limit are provided.</t>
+  </si>
+  <si>
+    <t>Overdraft limit is not a float.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is raised: "Overdraft limit must be a float."</t>
+    </r>
+  </si>
+  <si>
+    <t>Overdraft rate is not a float.</t>
+  </si>
+  <si>
+    <t>A ValueError is raised: "Overdraft rate must be a float."</t>
+  </si>
+  <si>
+    <t>Date created is not in the correct format (string).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>ValueError</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is raised: "Date created must be a string in 'YYYY-MM-DD' format."</t>
+    </r>
+  </si>
+  <si>
+    <t>Account balance exceeds the overdraft limit.</t>
+  </si>
+  <si>
+    <r>
+      <t>balance=1500.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_limit=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_rate=0.05</t>
+    </r>
+  </si>
+  <si>
+    <t>Service charges are calculated based on a standard fee with no overdraft penalty.</t>
+  </si>
+  <si>
+    <t>Account balance is below the overdraft limit.</t>
+  </si>
+  <si>
+    <r>
+      <t>balance=500.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_limit=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_rate=0.05</t>
+    </r>
+  </si>
+  <si>
+    <t>Service charges are calculated, including overdraft fees.</t>
+  </si>
+  <si>
+    <t>Account balance is exactly equal to the overdraft limit.</t>
+  </si>
+  <si>
+    <r>
+      <t>balance=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_limit=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_rate=0.05</t>
+    </r>
+  </si>
+  <si>
+    <t>Service charges are calculated based on standard fees, no overdraft penalty applies.</t>
+  </si>
+  <si>
+    <t>All attributes are set to valid values.</t>
+  </si>
+  <si>
+    <r>
+      <t>account_number=12345</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>balance=500.00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>__str__</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> returns: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>"Account Number: 12345 Balance: $500.00"</t>
+    </r>
+  </si>
+  <si>
+    <t>account_number=12345, client_number=67890, balance=500.00, overdraft_limit=1000.00, overdraft_rate=0.05, date_created="2023-01-01"</t>
+  </si>
+  <si>
+    <t>account_number=12345, client_number=67890, balance=500.00, overdraft_limit="invalid", overdraft_rate=0.05, date_created="2023-01-01"</t>
+  </si>
+  <si>
+    <r>
+      <t>account_number=12345</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>client_number=67890</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>balance=500.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_limit=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_rate="invalid"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>date_created="2023-01-01"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>account_number=12345</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>client_number=67890</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>balance=500.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_limit=1000.00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>overdraft_rate=0.05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>date_created=20230101</t>
+    </r>
+  </si>
+  <si>
+    <t>Attributes are successfully set: account_number=12345, client_number=67890, balance=500.00, overdraft_limit=1000.00, overdraft_rate=0.05, date_created="2023-01-01".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +761,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -555,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -583,9 +1041,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -609,6 +1064,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,53 +1619,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" customWidth="1"/>
+    <col min="6" max="6" width="77.88671875" customWidth="1"/>
+    <col min="7" max="7" width="48.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1"/>
+    <row r="2" spans="2:7" ht="73.2" customHeight="1" thickBot="1">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickBot="1">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1230,11 +1697,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1244,11 +1717,17 @@
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1258,11 +1737,17 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.2" customHeight="1">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1272,11 +1757,17 @@
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B11" s="3">
         <v>5</v>
       </c>
@@ -1286,11 +1777,17 @@
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1300,11 +1797,17 @@
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.2" customHeight="1">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1314,11 +1817,17 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1">
       <c r="B14" s="3">
         <v>8</v>
       </c>
@@ -1328,11 +1837,17 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1342,7 +1857,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="31.2" customHeight="1">
       <c r="B16" s="11">
         <v>10</v>
       </c>
@@ -1352,7 +1867,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -1362,7 +1877,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1372,7 +1887,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1382,7 +1897,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1392,7 +1907,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1402,7 +1917,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1412,7 +1927,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1422,7 +1937,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1432,7 +1947,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="31.2" customHeight="1">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1442,7 +1957,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B26" s="3">
         <v>20</v>
       </c>
@@ -1452,7 +1967,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1462,7 +1977,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.2" customHeight="1">
       <c r="B28" s="11">
         <v>22</v>
       </c>
@@ -1472,7 +1987,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B29" s="3">
         <v>23</v>
       </c>
@@ -1482,7 +1997,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.2" customHeight="1" thickBot="1">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1492,15 +2007,15 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+    <row r="32" spans="2:7">
+      <c r="B32" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1510,9 +2025,10 @@
     <mergeCell ref="B32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>